<commit_message>
Mostly picture data added
</commit_message>
<xml_diff>
--- a/src/sections/simple/Samling.xlsx
+++ b/src/sections/simple/Samling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olaveikrem/Documents/Inkunabulasjon-new/src/sections/simple/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223EC72E-E1A4-5948-A0CD-CD06C6ECB65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F7EA37-73AE-914C-8C53-9EAD80E89178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{55A60228-B19F-1F4D-92F6-862568A3AB42}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="217">
   <si>
     <t>Nummer</t>
   </si>
   <si>
-    <t>Tiitel</t>
-  </si>
-  <si>
     <t>Ark 1</t>
   </si>
   <si>
@@ -420,6 +417,276 @@
   </si>
   <si>
     <t>Bak59</t>
+  </si>
+  <si>
+    <t>Ark60</t>
+  </si>
+  <si>
+    <t>Bak60</t>
+  </si>
+  <si>
+    <t>Ark61</t>
+  </si>
+  <si>
+    <t>Bak61</t>
+  </si>
+  <si>
+    <t>Ark62</t>
+  </si>
+  <si>
+    <t>Bak62</t>
+  </si>
+  <si>
+    <t>Ark63</t>
+  </si>
+  <si>
+    <t>Bak63</t>
+  </si>
+  <si>
+    <t>Ark64</t>
+  </si>
+  <si>
+    <t>Bak64</t>
+  </si>
+  <si>
+    <t>Ark65</t>
+  </si>
+  <si>
+    <t>Bak65</t>
+  </si>
+  <si>
+    <t>Ark66</t>
+  </si>
+  <si>
+    <t>Bak66</t>
+  </si>
+  <si>
+    <t>Ark67</t>
+  </si>
+  <si>
+    <t>Bak67</t>
+  </si>
+  <si>
+    <t>Ark68</t>
+  </si>
+  <si>
+    <t>Bak68</t>
+  </si>
+  <si>
+    <t>Ark69</t>
+  </si>
+  <si>
+    <t>Bak69</t>
+  </si>
+  <si>
+    <t>Ark70</t>
+  </si>
+  <si>
+    <t>Bak70</t>
+  </si>
+  <si>
+    <t>Ark71</t>
+  </si>
+  <si>
+    <t>Bak71</t>
+  </si>
+  <si>
+    <t>Ark72</t>
+  </si>
+  <si>
+    <t>Bak72</t>
+  </si>
+  <si>
+    <t>Ark73</t>
+  </si>
+  <si>
+    <t>Bak73</t>
+  </si>
+  <si>
+    <t>Ark74</t>
+  </si>
+  <si>
+    <t>Bak74</t>
+  </si>
+  <si>
+    <t>Ark75</t>
+  </si>
+  <si>
+    <t>Bak75</t>
+  </si>
+  <si>
+    <t>Ark76</t>
+  </si>
+  <si>
+    <t>Bak76</t>
+  </si>
+  <si>
+    <t>Ark77</t>
+  </si>
+  <si>
+    <t>Bak77</t>
+  </si>
+  <si>
+    <t>Ark78</t>
+  </si>
+  <si>
+    <t>Bak78</t>
+  </si>
+  <si>
+    <t>Ark79</t>
+  </si>
+  <si>
+    <t>Bak79</t>
+  </si>
+  <si>
+    <t>Ark80</t>
+  </si>
+  <si>
+    <t>Bak80</t>
+  </si>
+  <si>
+    <t>Ark81</t>
+  </si>
+  <si>
+    <t>Bak81</t>
+  </si>
+  <si>
+    <t>Ark82</t>
+  </si>
+  <si>
+    <t>Bak82</t>
+  </si>
+  <si>
+    <t>Ark83</t>
+  </si>
+  <si>
+    <t>Bak83</t>
+  </si>
+  <si>
+    <t>Ark84</t>
+  </si>
+  <si>
+    <t>Bak84</t>
+  </si>
+  <si>
+    <t>Ark85</t>
+  </si>
+  <si>
+    <t>Bak85</t>
+  </si>
+  <si>
+    <t>Ark86</t>
+  </si>
+  <si>
+    <t>Bak86</t>
+  </si>
+  <si>
+    <t>Ark87</t>
+  </si>
+  <si>
+    <t>Bak87</t>
+  </si>
+  <si>
+    <t>Ark88</t>
+  </si>
+  <si>
+    <t>Bak88</t>
+  </si>
+  <si>
+    <t>Ark89</t>
+  </si>
+  <si>
+    <t>Bak89</t>
+  </si>
+  <si>
+    <t>Ark90</t>
+  </si>
+  <si>
+    <t>Bak90</t>
+  </si>
+  <si>
+    <t>Ark91</t>
+  </si>
+  <si>
+    <t>Bak91</t>
+  </si>
+  <si>
+    <t>Ark92</t>
+  </si>
+  <si>
+    <t>Bak92</t>
+  </si>
+  <si>
+    <t>Ark93</t>
+  </si>
+  <si>
+    <t>Bak93</t>
+  </si>
+  <si>
+    <t>Ark94</t>
+  </si>
+  <si>
+    <t>Bak94</t>
+  </si>
+  <si>
+    <t>Ark95</t>
+  </si>
+  <si>
+    <t>Bak95</t>
+  </si>
+  <si>
+    <t>Ark96</t>
+  </si>
+  <si>
+    <t>Bak96</t>
+  </si>
+  <si>
+    <t>Ark97</t>
+  </si>
+  <si>
+    <t>Bak97</t>
+  </si>
+  <si>
+    <t>Ark98</t>
+  </si>
+  <si>
+    <t>Bak98</t>
+  </si>
+  <si>
+    <t>Ark99</t>
+  </si>
+  <si>
+    <t>Bak99</t>
+  </si>
+  <si>
+    <t>Ark100</t>
+  </si>
+  <si>
+    <t>Bak100</t>
+  </si>
+  <si>
+    <t>Ark101</t>
+  </si>
+  <si>
+    <t>Bak101</t>
+  </si>
+  <si>
+    <t>Ark102</t>
+  </si>
+  <si>
+    <t>Bak102</t>
+  </si>
+  <si>
+    <t>Ark103</t>
+  </si>
+  <si>
+    <t>Bak103</t>
+  </si>
+  <si>
+    <t>Tittel</t>
+  </si>
+  <si>
+    <t>Aar</t>
   </si>
 </sst>
 </file>
@@ -777,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40BFC11-D50C-734F-8B28-CCF364789754}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,324 +1055,327 @@
     <col min="6" max="6" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>215</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
       <c r="F6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1113,19 +1383,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1133,19 +1403,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1153,19 +1423,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1173,19 +1443,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1193,19 +1463,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1213,19 +1483,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
         <v>50</v>
       </c>
-      <c r="C22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>51</v>
-      </c>
       <c r="F22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1233,19 +1503,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
         <v>52</v>
       </c>
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
-        <v>53</v>
-      </c>
       <c r="F23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1253,19 +1523,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
         <v>54</v>
       </c>
-      <c r="C24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" t="s">
-        <v>55</v>
-      </c>
       <c r="F24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1273,19 +1543,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
         <v>56</v>
       </c>
-      <c r="C25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>57</v>
-      </c>
       <c r="F25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1293,19 +1563,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
         <v>58</v>
       </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" t="s">
-        <v>59</v>
-      </c>
       <c r="F26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1313,19 +1583,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
         <v>60</v>
       </c>
-      <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>61</v>
-      </c>
       <c r="F27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1333,19 +1603,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
         <v>62</v>
       </c>
-      <c r="C28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" t="s">
-        <v>63</v>
-      </c>
       <c r="F28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1353,19 +1623,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
         <v>64</v>
       </c>
-      <c r="C29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" t="s">
-        <v>65</v>
-      </c>
       <c r="F29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1373,19 +1643,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
         <v>66</v>
       </c>
-      <c r="C30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" t="s">
-        <v>67</v>
-      </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1393,19 +1663,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
         <v>68</v>
       </c>
-      <c r="C31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>69</v>
-      </c>
       <c r="F31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1413,19 +1683,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
         <v>70</v>
       </c>
-      <c r="C32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" t="s">
-        <v>71</v>
-      </c>
       <c r="F32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1433,19 +1703,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
         <v>72</v>
       </c>
-      <c r="C33" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" t="s">
-        <v>73</v>
-      </c>
       <c r="F33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1453,19 +1723,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
         <v>74</v>
       </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" t="s">
-        <v>75</v>
-      </c>
       <c r="F34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1473,19 +1743,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
         <v>76</v>
       </c>
-      <c r="C35" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>77</v>
-      </c>
       <c r="F35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1493,19 +1763,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
         <v>78</v>
       </c>
-      <c r="C36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" t="s">
-        <v>79</v>
-      </c>
       <c r="F36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1513,19 +1783,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
         <v>80</v>
       </c>
-      <c r="C37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>81</v>
-      </c>
       <c r="F37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1533,19 +1803,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
         <v>82</v>
       </c>
-      <c r="C38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" t="s">
-        <v>83</v>
-      </c>
       <c r="F38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1553,19 +1823,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
         <v>84</v>
       </c>
-      <c r="C39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" t="s">
-        <v>85</v>
-      </c>
       <c r="F39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1573,19 +1843,19 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" t="s">
         <v>86</v>
       </c>
-      <c r="C40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" t="s">
-        <v>87</v>
-      </c>
       <c r="F40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1593,19 +1863,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
         <v>88</v>
       </c>
-      <c r="C41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" t="s">
-        <v>89</v>
-      </c>
       <c r="F41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1613,19 +1883,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" t="s">
         <v>90</v>
       </c>
-      <c r="C42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" t="s">
-        <v>91</v>
-      </c>
       <c r="F42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1633,19 +1903,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
         <v>92</v>
       </c>
-      <c r="C43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" t="s">
-        <v>93</v>
-      </c>
       <c r="F43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1653,19 +1923,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" t="s">
         <v>94</v>
       </c>
-      <c r="C44" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" t="s">
-        <v>95</v>
-      </c>
       <c r="F44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1673,19 +1943,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
         <v>96</v>
       </c>
-      <c r="C45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" t="s">
-        <v>97</v>
-      </c>
       <c r="F45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1693,19 +1963,19 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
         <v>98</v>
       </c>
-      <c r="C46" t="s">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" t="s">
-        <v>99</v>
-      </c>
       <c r="F46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1713,19 +1983,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" t="s">
         <v>100</v>
       </c>
-      <c r="C47" t="s">
-        <v>2</v>
-      </c>
-      <c r="D47" t="s">
-        <v>6</v>
-      </c>
-      <c r="E47" t="s">
-        <v>101</v>
-      </c>
       <c r="F47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1733,19 +2003,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
         <v>102</v>
       </c>
-      <c r="C48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D48" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" t="s">
-        <v>103</v>
-      </c>
       <c r="F48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1753,19 +2023,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" t="s">
         <v>104</v>
       </c>
-      <c r="C49" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" t="s">
-        <v>105</v>
-      </c>
       <c r="F49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1773,19 +2043,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
         <v>106</v>
       </c>
-      <c r="C50" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" t="s">
-        <v>107</v>
-      </c>
       <c r="F50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1793,19 +2063,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" t="s">
         <v>108</v>
       </c>
-      <c r="C51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D51" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" t="s">
-        <v>109</v>
-      </c>
       <c r="F51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1813,19 +2083,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
         <v>110</v>
       </c>
-      <c r="C52" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" t="s">
-        <v>5</v>
-      </c>
-      <c r="E52" t="s">
-        <v>111</v>
-      </c>
       <c r="F52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1833,19 +2103,19 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" t="s">
         <v>112</v>
       </c>
-      <c r="C53" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" t="s">
-        <v>113</v>
-      </c>
       <c r="F53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1853,19 +2123,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" t="s">
         <v>114</v>
       </c>
-      <c r="C54" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54" t="s">
-        <v>5</v>
-      </c>
-      <c r="E54" t="s">
-        <v>115</v>
-      </c>
       <c r="F54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1873,19 +2143,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" t="s">
         <v>116</v>
       </c>
-      <c r="C55" t="s">
-        <v>2</v>
-      </c>
-      <c r="D55" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" t="s">
-        <v>117</v>
-      </c>
       <c r="F55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -1893,19 +2163,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
         <v>118</v>
       </c>
-      <c r="C56" t="s">
-        <v>2</v>
-      </c>
-      <c r="D56" t="s">
-        <v>5</v>
-      </c>
-      <c r="E56" t="s">
-        <v>119</v>
-      </c>
       <c r="F56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1913,19 +2183,19 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" t="s">
         <v>120</v>
       </c>
-      <c r="C57" t="s">
-        <v>2</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" t="s">
-        <v>121</v>
-      </c>
       <c r="F57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -1933,19 +2203,19 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s">
         <v>122</v>
       </c>
-      <c r="C58" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58" t="s">
-        <v>5</v>
-      </c>
-      <c r="E58" t="s">
-        <v>123</v>
-      </c>
       <c r="F58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -1953,19 +2223,19 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
         <v>124</v>
       </c>
-      <c r="C59" t="s">
-        <v>2</v>
-      </c>
-      <c r="D59" t="s">
-        <v>6</v>
-      </c>
-      <c r="E59" t="s">
-        <v>125</v>
-      </c>
       <c r="F59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -1973,19 +2243,899 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" t="s">
         <v>126</v>
       </c>
-      <c r="C60" t="s">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s">
-        <v>5</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
         <v>127</v>
       </c>
-      <c r="F60" t="s">
-        <v>49</v>
+      <c r="C61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>130</v>
+      </c>
+      <c r="F62" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" t="s">
+        <v>132</v>
+      </c>
+      <c r="F63" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" t="s">
+        <v>134</v>
+      </c>
+      <c r="F64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" t="s">
+        <v>136</v>
+      </c>
+      <c r="F65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" t="s">
+        <v>138</v>
+      </c>
+      <c r="F66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" t="s">
+        <v>140</v>
+      </c>
+      <c r="F67" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>141</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68" t="s">
+        <v>142</v>
+      </c>
+      <c r="F68" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" t="s">
+        <v>144</v>
+      </c>
+      <c r="F69" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>145</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" t="s">
+        <v>146</v>
+      </c>
+      <c r="F70" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" t="s">
+        <v>148</v>
+      </c>
+      <c r="F71" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" t="s">
+        <v>150</v>
+      </c>
+      <c r="F72" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73" t="s">
+        <v>152</v>
+      </c>
+      <c r="F73" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>153</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
+        <v>5</v>
+      </c>
+      <c r="E74" t="s">
+        <v>154</v>
+      </c>
+      <c r="F74" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" t="s">
+        <v>156</v>
+      </c>
+      <c r="F75" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>157</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" t="s">
+        <v>158</v>
+      </c>
+      <c r="F76" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>159</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" t="s">
+        <v>160</v>
+      </c>
+      <c r="F77" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>161</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1</v>
+      </c>
+      <c r="D78" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" t="s">
+        <v>162</v>
+      </c>
+      <c r="F78" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>163</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" t="s">
+        <v>164</v>
+      </c>
+      <c r="F79" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>165</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>5</v>
+      </c>
+      <c r="E80" t="s">
+        <v>166</v>
+      </c>
+      <c r="F80" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>167</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81" t="s">
+        <v>168</v>
+      </c>
+      <c r="F81" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>169</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" t="s">
+        <v>170</v>
+      </c>
+      <c r="F82" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>171</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83" t="s">
+        <v>4</v>
+      </c>
+      <c r="E83" t="s">
+        <v>172</v>
+      </c>
+      <c r="F83" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>173</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E84" t="s">
+        <v>174</v>
+      </c>
+      <c r="F84" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" t="s">
+        <v>176</v>
+      </c>
+      <c r="F85" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>177</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" t="s">
+        <v>178</v>
+      </c>
+      <c r="F86" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>179</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>4</v>
+      </c>
+      <c r="E87" t="s">
+        <v>180</v>
+      </c>
+      <c r="F87" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>181</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88" t="s">
+        <v>5</v>
+      </c>
+      <c r="E88" t="s">
+        <v>182</v>
+      </c>
+      <c r="F88" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>183</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89" t="s">
+        <v>4</v>
+      </c>
+      <c r="E89" t="s">
+        <v>184</v>
+      </c>
+      <c r="F89" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>185</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>5</v>
+      </c>
+      <c r="E90" t="s">
+        <v>186</v>
+      </c>
+      <c r="F90" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>187</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>4</v>
+      </c>
+      <c r="E91" t="s">
+        <v>188</v>
+      </c>
+      <c r="F91" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>189</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92" t="s">
+        <v>5</v>
+      </c>
+      <c r="E92" t="s">
+        <v>190</v>
+      </c>
+      <c r="F92" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>191</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93" t="s">
+        <v>4</v>
+      </c>
+      <c r="E93" t="s">
+        <v>192</v>
+      </c>
+      <c r="F93" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>193</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1</v>
+      </c>
+      <c r="D94" t="s">
+        <v>5</v>
+      </c>
+      <c r="E94" t="s">
+        <v>194</v>
+      </c>
+      <c r="F94" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>195</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95" t="s">
+        <v>4</v>
+      </c>
+      <c r="E95" t="s">
+        <v>196</v>
+      </c>
+      <c r="F95" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>197</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>5</v>
+      </c>
+      <c r="E96" t="s">
+        <v>198</v>
+      </c>
+      <c r="F96" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>199</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>4</v>
+      </c>
+      <c r="E97" t="s">
+        <v>200</v>
+      </c>
+      <c r="F97" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>201</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" t="s">
+        <v>5</v>
+      </c>
+      <c r="E98" t="s">
+        <v>202</v>
+      </c>
+      <c r="F98" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>203</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99" t="s">
+        <v>4</v>
+      </c>
+      <c r="E99" t="s">
+        <v>204</v>
+      </c>
+      <c r="F99" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>205</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1</v>
+      </c>
+      <c r="D100" t="s">
+        <v>5</v>
+      </c>
+      <c r="E100" t="s">
+        <v>206</v>
+      </c>
+      <c r="F100" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>207</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1</v>
+      </c>
+      <c r="D101" t="s">
+        <v>4</v>
+      </c>
+      <c r="E101" t="s">
+        <v>208</v>
+      </c>
+      <c r="F101" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>209</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1</v>
+      </c>
+      <c r="D102" t="s">
+        <v>5</v>
+      </c>
+      <c r="E102" t="s">
+        <v>210</v>
+      </c>
+      <c r="F102" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>211</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1</v>
+      </c>
+      <c r="D103" t="s">
+        <v>4</v>
+      </c>
+      <c r="E103" t="s">
+        <v>212</v>
+      </c>
+      <c r="F103" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>213</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1</v>
+      </c>
+      <c r="D104" t="s">
+        <v>5</v>
+      </c>
+      <c r="E104" t="s">
+        <v>214</v>
+      </c>
+      <c r="F104" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>